<commit_message>
updated FDANDC->FDANationalDrugCode, updated EOBProfileComparison xlsx and png, EOBPharmacy
</commit_message>
<xml_diff>
--- a/fsh/ig-data/input/images/EOBProfileComparison20200929.xlsx
+++ b/fsh/ig-data/input/images/EOBProfileComparison20200929.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/carin-bb/fsh/ig-data/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A494F679-5F1D-E240-88B4-EFC9350C935A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41215AC4-7C6F-D147-BE22-1F14C65E628E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7700" yWindow="860" windowWidth="38720" windowHeight="24740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>detail.productOrService</t>
   </si>
   <si>
-    <t>FDANDC</t>
-  </si>
-  <si>
     <t>Invariant enforces type of reference based on role careteam.role code</t>
   </si>
   <si>
@@ -475,6 +472,9 @@
   </si>
   <si>
     <t>C4BBSupportingInfoType</t>
+  </si>
+  <si>
+    <t>FDANationalDrugCode</t>
   </si>
 </sst>
 </file>
@@ -1559,8 +1559,8 @@
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1584,19 +1584,19 @@
         <v>5</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>74</v>
-      </c>
       <c r="G1" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>0</v>
@@ -1609,34 +1609,34 @@
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
       <c r="D2" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>72</v>
-      </c>
       <c r="H2" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="37"/>
@@ -1663,13 +1663,13 @@
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="G5" s="37" t="s">
         <v>119</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>120</v>
       </c>
       <c r="H5" s="38"/>
     </row>
@@ -1681,13 +1681,13 @@
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H6" s="21"/>
     </row>
@@ -1697,11 +1697,11 @@
         <v>8</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="28"/>
       <c r="E7" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
@@ -1709,14 +1709,14 @@
     </row>
     <row r="8" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="44" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>40</v>
       </c>
       <c r="C8" s="44"/>
       <c r="D8" s="44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="45"/>
       <c r="F8" s="45"/>
@@ -1733,7 +1733,7 @@
       <c r="C9" s="37"/>
       <c r="D9" s="49"/>
       <c r="E9" s="49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F9" s="49"/>
       <c r="G9" s="49"/>
@@ -1747,7 +1747,7 @@
       <c r="C10" s="32"/>
       <c r="D10" s="53"/>
       <c r="E10" s="53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F10" s="53"/>
       <c r="G10" s="53"/>
@@ -1755,12 +1755,12 @@
     </row>
     <row r="11" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="56"/>
       <c r="C11" s="56"/>
       <c r="D11" s="56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="57"/>
       <c r="F11" s="57"/>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="60"/>
       <c r="F12" s="60"/>
@@ -1789,10 +1789,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E13" s="62"/>
       <c r="F13" s="62"/>
@@ -1809,53 +1809,53 @@
       <c r="C14" s="59"/>
       <c r="D14" s="59"/>
       <c r="E14" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="F14" s="59" t="s">
-        <v>121</v>
-      </c>
-      <c r="G14" s="59" t="s">
+      <c r="H14" s="65" t="s">
         <v>122</v>
-      </c>
-      <c r="H14" s="65" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
       <c r="B15" s="77" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="77"/>
       <c r="D15" s="77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G15" s="77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H15" s="78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="66"/>
       <c r="B16" s="79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="79" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D16" s="79"/>
       <c r="E16" s="79"/>
       <c r="F16" s="79"/>
       <c r="G16" s="79" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H16" s="80"/>
     </row>
@@ -1866,29 +1866,29 @@
       <c r="B17" s="81"/>
       <c r="C17" s="81"/>
       <c r="D17" s="81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="81" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" s="81" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G17" s="82"/>
       <c r="H17" s="83"/>
     </row>
     <row r="18" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="93" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="100" t="s">
         <v>145</v>
-      </c>
-      <c r="C18" s="93" t="s">
-        <v>114</v>
-      </c>
-      <c r="D18" s="100" t="s">
-        <v>146</v>
       </c>
       <c r="E18" s="93"/>
       <c r="F18" s="93"/>
@@ -1898,45 +1898,45 @@
     <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="23"/>
       <c r="B19" s="84" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="84" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D19" s="84"/>
       <c r="E19" s="84" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F19" s="84" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G19" s="84" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H19" s="85" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23"/>
       <c r="B20" s="77" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D20" s="77"/>
       <c r="E20" s="77"/>
       <c r="F20" s="77"/>
       <c r="G20" s="77" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H20" s="78"/>
     </row>
     <row r="21" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="23"/>
       <c r="B21" s="86" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C21" s="86"/>
       <c r="D21" s="86"/>
@@ -1956,17 +1956,17 @@
     <row r="22" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="23"/>
       <c r="B22" s="77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="77" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="77"/>
       <c r="E22" s="77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F22" s="77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G22" s="77"/>
       <c r="H22" s="78"/>
@@ -1974,17 +1974,17 @@
     <row r="23" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="23"/>
       <c r="B23" s="86" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="86" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="86"/>
       <c r="E23" s="86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F23" s="86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G23" s="86"/>
       <c r="H23" s="87"/>
@@ -1992,17 +1992,17 @@
     <row r="24" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="23"/>
       <c r="B24" s="77" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="77" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="77"/>
       <c r="E24" s="77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F24" s="77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G24" s="77"/>
       <c r="H24" s="78"/>
@@ -2010,17 +2010,17 @@
     <row r="25" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="23"/>
       <c r="B25" s="86" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="86" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="86"/>
       <c r="E25" s="86" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F25" s="86" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G25" s="86"/>
       <c r="H25" s="87"/>
@@ -2028,12 +2028,12 @@
     <row r="26" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="23"/>
       <c r="B26" s="77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="77"/>
       <c r="D26" s="77"/>
       <c r="E26" s="77" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F26" s="77"/>
       <c r="G26" s="77"/>
@@ -2042,39 +2042,39 @@
     <row r="27" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="23"/>
       <c r="B27" s="86" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="86" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D27" s="86"/>
       <c r="E27" s="86"/>
       <c r="F27" s="86"/>
       <c r="G27" s="86"/>
       <c r="H27" s="87" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="23"/>
       <c r="B28" s="77" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C28" s="77" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D28" s="77"/>
       <c r="E28" s="77"/>
       <c r="F28" s="77"/>
       <c r="G28" s="77"/>
       <c r="H28" s="78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="23"/>
       <c r="B29" s="86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" s="86"/>
       <c r="D29" s="86"/>
@@ -2088,39 +2088,39 @@
     <row r="30" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="23"/>
       <c r="B30" s="77" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="77" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D30" s="77"/>
       <c r="E30" s="77"/>
       <c r="F30" s="77"/>
       <c r="G30" s="77"/>
       <c r="H30" s="78" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="23"/>
       <c r="B31" s="86" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="86" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" s="86"/>
       <c r="E31" s="86"/>
       <c r="F31" s="86"/>
       <c r="G31" s="86"/>
       <c r="H31" s="87" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="23"/>
       <c r="B32" s="77" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="77"/>
       <c r="D32" s="77"/>
@@ -2134,12 +2134,12 @@
     <row r="33" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="23"/>
       <c r="B33" s="86" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="86"/>
       <c r="D33" s="86"/>
       <c r="E33" s="86" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F33" s="86"/>
       <c r="G33" s="86"/>
@@ -2148,29 +2148,29 @@
     <row r="34" spans="1:8" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="69"/>
       <c r="B34" s="88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" s="88"/>
       <c r="D34" s="88"/>
       <c r="E34" s="88"/>
       <c r="F34" s="88"/>
       <c r="G34" s="88" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H34" s="89"/>
     </row>
     <row r="35" spans="1:8" ht="26" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="70" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" s="90" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="90" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D35" s="90" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E35" s="90"/>
       <c r="F35" s="90"/>
@@ -2179,62 +2179,62 @@
     </row>
     <row r="36" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="71" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" s="93" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C36" s="93"/>
       <c r="D36" s="93"/>
       <c r="E36" s="93" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F36" s="93" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G36" s="93" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H36" s="94" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="72"/>
       <c r="B37" s="79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="79" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D37" s="79"/>
       <c r="E37" s="79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F37" s="79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G37" s="79"/>
       <c r="H37" s="80" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B38" s="93" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C38" s="93" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D38" s="93"/>
       <c r="E38" s="93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F38" s="93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G38" s="93"/>
       <c r="H38" s="94"/>
@@ -2242,35 +2242,35 @@
     <row r="39" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="69"/>
       <c r="B39" s="79" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" s="79"/>
       <c r="D39" s="79"/>
       <c r="E39" s="79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F39" s="79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G39" s="95"/>
       <c r="H39" s="96"/>
     </row>
     <row r="40" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40" s="93" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="93" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D40" s="93"/>
       <c r="E40" s="93" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F40" s="93" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G40" s="93"/>
       <c r="H40" s="94"/>
@@ -2281,17 +2281,17 @@
         <v>15</v>
       </c>
       <c r="C41" s="86" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D41" s="86"/>
       <c r="E41" s="86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F41" s="86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G41" s="86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H41" s="87"/>
     </row>
@@ -2301,29 +2301,29 @@
         <v>16</v>
       </c>
       <c r="C42" s="77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D42" s="77"/>
       <c r="E42" s="77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F42" s="77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G42" s="77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H42" s="78" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="24"/>
       <c r="B43" s="86" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C43" s="86" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D43" s="86"/>
       <c r="E43" s="86"/>
@@ -2339,24 +2339,24 @@
         <v>19</v>
       </c>
       <c r="C44" s="77" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D44" s="77"/>
       <c r="E44" s="77"/>
       <c r="F44" s="77"/>
       <c r="G44" s="77"/>
       <c r="H44" s="78" t="s">
-        <v>20</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="74"/>
       <c r="B45" s="79" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C45" s="79"/>
       <c r="D45" s="79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E45" s="95"/>
       <c r="F45" s="95"/>
@@ -2365,66 +2365,66 @@
     </row>
     <row r="46" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B46" s="93" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C46" s="93" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D46" s="93"/>
       <c r="E46" s="93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F46" s="93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G46" s="93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H46" s="94" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="25"/>
       <c r="B47" s="86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C47" s="86"/>
       <c r="D47" s="86"/>
       <c r="E47" s="86"/>
       <c r="F47" s="86"/>
       <c r="G47" s="86" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H47" s="87"/>
     </row>
     <row r="48" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="25"/>
       <c r="B48" s="77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C48" s="77"/>
       <c r="D48" s="77"/>
       <c r="E48" s="77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F48" s="77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G48" s="77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H48" s="78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="26"/>
       <c r="B49" s="79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49" s="79"/>
       <c r="D49" s="79"/>
@@ -2441,14 +2441,14 @@
     </row>
     <row r="50" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="75" t="s">
         <v>88</v>
-      </c>
-      <c r="B50" s="75" t="s">
-        <v>89</v>
       </c>
       <c r="C50" s="75"/>
       <c r="D50" s="75" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E50" s="75"/>
       <c r="F50" s="75"/>
@@ -2496,24 +2496,24 @@
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2523,7 +2523,7 @@
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -2532,7 +2532,7 @@
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -2541,61 +2541,61 @@
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -2605,7 +2605,7 @@
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -2614,18 +2614,18 @@
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -2634,17 +2634,17 @@
     <row r="14" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -2654,7 +2654,7 @@
     <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -2663,7 +2663,7 @@
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -2672,7 +2672,7 @@
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -2681,7 +2681,7 @@
     <row r="19" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
       <c r="B19" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -2689,7 +2689,7 @@
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -2699,7 +2699,7 @@
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -2708,7 +2708,7 @@
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>

</xml_diff>